<commit_message>
Implement API call changes. No direct API for FluSurv-NET has been found. RESP-NET only provides nation-wide results.
</commit_message>
<xml_diff>
--- a/Data Pull/Support Functions/Nuanced Import Simulation/Data Dictionary_RESP-NET Programs_copied 03.30.2025.xlsx
+++ b/Data Pull/Support Functions/Nuanced Import Simulation/Data Dictionary_RESP-NET Programs_copied 03.30.2025.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sg2736/Desktop/DSDE/Projects/YSPH-DSDE Repos/data.gov Curation and Visualization/data-gov-archiving-and-harmonization/Data Pull/Support Functions/Nuanced Inport Simulation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sg2736/Desktop/DSDE/Projects/YSPH-DSDE Repos/data.gov Curation and Visualization/data-gov-archiving-and-harmonization/Data Pull/Support Functions/Nuanced Import Simulation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC593184-8ACF-AC4A-B5B0-33B7031E0BD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5530460A-FE87-954B-8D5F-B7C1F98232CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6920" yWindow="760" windowWidth="23320" windowHeight="17440" activeTab="2" xr2:uid="{54E2C9C4-A07C-D649-8B51-A72E6770E04B}"/>
+    <workbookView xWindow="31600" yWindow="500" windowWidth="29820" windowHeight="20020" xr2:uid="{54E2C9C4-A07C-D649-8B51-A72E6770E04B}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="4" r:id="rId1"/>
@@ -752,8 +752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76F607C6-73D5-B14E-A6AF-691B2E044AB1}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -876,7 +876,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -913,7 +913,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{380EAF19-A938-084D-AA6B-995A35679FAA}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add function updates for data pull step.
</commit_message>
<xml_diff>
--- a/Data Pull/Support Functions/Nuanced Import Simulation/Data Dictionary_RESP-NET Programs_copied 03.30.2025.xlsx
+++ b/Data Pull/Support Functions/Nuanced Import Simulation/Data Dictionary_RESP-NET Programs_copied 03.30.2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sg2736/Desktop/DSDE/Projects/YSPH-DSDE Repos/data.gov Curation and Visualization/data-gov-archiving-and-harmonization/Data Pull/Support Functions/Nuanced Import Simulation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5530460A-FE87-954B-8D5F-B7C1F98232CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1DD5BE7-024B-5842-9064-F4B44F7614D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31600" yWindow="500" windowWidth="29820" windowHeight="20020" xr2:uid="{54E2C9C4-A07C-D649-8B51-A72E6770E04B}"/>
+    <workbookView xWindow="31600" yWindow="500" windowWidth="29820" windowHeight="20020" activeTab="2" xr2:uid="{54E2C9C4-A07C-D649-8B51-A72E6770E04B}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="4" r:id="rId1"/>
@@ -752,8 +752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76F607C6-73D5-B14E-A6AF-691B2E044AB1}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -913,8 +913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{380EAF19-A938-084D-AA6B-995A35679FAA}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>